<commit_message>
update private request test case
</commit_message>
<xml_diff>
--- a/tests/xlsx_requests/private_request/private_request_translate.xlsx
+++ b/tests/xlsx_requests/private_request/private_request_translate.xlsx
@@ -116,14 +116,15 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="D38" authorId="0">
+    <comment ref="B38" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Sends key strokes to an input element</t>
+          <t xml:space="preserve">Installed addon: File Upload
+With this addon you can upload attachments and files to your web application. Just select the applicable element and pick the file upload action.</t>
         </d:r>
       </text>
     </comment>
@@ -154,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t/>
   </si>
@@ -216,7 +217,7 @@
     <t>Last Modified on</t>
   </si>
   <si>
-    <t>04/22/2022 15:58:59</t>
+    <t>04/22/2022 16:15:35</t>
   </si>
   <si>
     <t>Web Application</t>
@@ -384,13 +385,16 @@
     <t>Button: TÌM TỆP TRÊN MÁY TÍNH CỦA BẠN (located by XPATH: //span[. = 'Tìm tệp trên máy tính của bạn'])</t>
   </si>
   <si>
-    <t>Type 'C:\fakepath\test_file_2.xlsx' in 'contained-button-file' (Generic Web Element)</t>
+    <t>Uploads a file to a given element with the 'file' type</t>
+  </si>
+  <si>
+    <t>Upload file</t>
   </si>
   <si>
     <t>Generic Web Element: contained-button-file (located by XPATH: //input)</t>
   </si>
   <si>
-    <t>keys=C:\fakepath\test_file_2.xlsx</t>
+    <t>PATH=/home/nam/Workspace/KC4.0_DichDaNgu_FrontEnd/tests/xlsx_requests/test_files/test_file_2.xlsx</t>
   </si>
   <si>
     <t>Click 'DỊCH' (Button)</t>
@@ -589,7 +593,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestParameters_Kj9pEWoQ" displayName="TestParameters_Kj9pEWoQ" ref="A22:D25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestParameters_ocCFho4s" displayName="TestParameters_ocCFho4s" ref="A22:D25">
   <autoFilter ref="A22:D25"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Name"/>
@@ -602,7 +606,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Steps_8Kgioymj" displayName="Steps_8Kgioymj" ref="A28:O40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Steps_Jc0nReQu" displayName="Steps_Jc0nReQu" ref="A28:O40">
   <autoFilter ref="A28:O40"/>
   <tableColumns count="15">
     <tableColumn id="1" name="#"/>
@@ -634,7 +638,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85714340209961" customWidth="1"/>
-    <col min="2" max="2" width="89.14286041259766" customWidth="1"/>
+    <col min="2" max="2" width="68.71428680419922" customWidth="1"/>
     <col min="3" max="3" width="14.25" customWidth="1"/>
     <col min="4" max="4" width="24.571428298950195" customWidth="1"/>
     <col min="5" max="5" width="114.57142639160156" customWidth="1"/>
@@ -643,7 +647,7 @@
     <col min="8" max="8" width="21.285715103149414" customWidth="1"/>
     <col min="9" max="9" width="14.821428298950195" customWidth="1"/>
     <col min="10" max="10" width="11.535714149475098" customWidth="1"/>
-    <col min="11" max="11" width="37.28571319580078" customWidth="1"/>
+    <col min="11" max="11" width="113.28571319580078" customWidth="1"/>
     <col min="12" max="12" width="11.392857551574707" customWidth="1"/>
     <col min="13" max="13" width="13.964285850524902" customWidth="1"/>
     <col min="14" max="14" width="14.392857551574707" customWidth="1"/>
@@ -1311,10 +1315,10 @@
         <v>76</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>55</v>
@@ -1332,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L38" s="0" t="s">
         <v>0</v>
@@ -1352,13 +1356,13 @@
         <v>11</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>53</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>55</v>
@@ -1396,14 +1400,14 @@
         <v>12</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>55</v>

</xml_diff>